<commit_message>
change the format in which the search results are returned
</commit_message>
<xml_diff>
--- a/SprintBacklog.xlsx
+++ b/SprintBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC951CF0-AE83-4193-BE2F-B1C044A3431C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A525CC-7CCB-4817-AF41-7A3192A65636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>Create results page for website to return list</t>
   </si>
   <si>
-    <t>Return list from database in order of provider ID</t>
-  </si>
-  <si>
     <t>9. As a customer, I can view search results on a map</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>AR, WM,AI</t>
   </si>
   <si>
-    <t>Return list from database from nearest to location</t>
-  </si>
-  <si>
     <t>12. As a customer, I can view details of a search result in the list</t>
   </si>
   <si>
@@ -231,6 +225,12 @@
   </si>
   <si>
     <t>User Story #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return list from database in order of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return list from database based on </t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +275,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -330,6 +336,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,8 +1035,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>33</v>
+      <c r="A22" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
@@ -1049,7 +1056,7 @@
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1">
         <v>8</v>
@@ -1057,10 +1064,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
         <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>36</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1093,8 +1100,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>37</v>
+      <c r="A26" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
@@ -1114,7 +1121,7 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1">
         <v>7</v>
@@ -1122,7 +1129,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
@@ -1139,7 +1146,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
         <v>21</v>
@@ -1159,7 +1166,7 @@
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1">
         <v>6</v>
@@ -1167,7 +1174,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -1184,7 +1191,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -1204,7 +1211,7 @@
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1">
         <v>6</v>
@@ -1212,7 +1219,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
@@ -1229,7 +1236,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
@@ -1249,7 +1256,7 @@
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1">
         <v>5</v>
@@ -1257,7 +1264,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -1274,7 +1281,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
@@ -1294,7 +1301,7 @@
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
@@ -1302,10 +1309,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -1339,7 +1346,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
         <v>21</v>
@@ -1359,7 +1366,7 @@
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1">
         <v>4</v>
@@ -1367,10 +1374,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D44" t="s">
         <v>14</v>
@@ -1404,7 +1411,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
         <v>21</v>
@@ -1424,7 +1431,7 @@
     </row>
     <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1">
         <v>4</v>
@@ -1432,10 +1439,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
         <v>14</v>
@@ -1455,7 +1462,7 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
         <v>26</v>
@@ -1472,7 +1479,7 @@
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1">
         <v>2</v>
@@ -1480,7 +1487,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D51" t="s">
         <v>14</v>
@@ -1497,10 +1504,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D52" t="s">
         <v>26</v>
@@ -1517,7 +1524,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
         <v>19</v>
@@ -1534,7 +1541,7 @@
     </row>
     <row r="54" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E54" s="9">
         <f t="shared" ref="E54:J54" si="0">SUM(E3:E53)</f>
@@ -1627,10 +1634,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -1662,7 +1669,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1677,7 +1684,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1695,7 +1702,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1710,7 +1717,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1725,7 +1732,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1740,7 +1747,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
fix sprint backlog task definitions
</commit_message>
<xml_diff>
--- a/SprintBacklog.xlsx
+++ b/SprintBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A525CC-7CCB-4817-AF41-7A3192A65636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F11304-CC38-4936-88D1-2F1D1B1FD7C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="67">
   <si>
     <t>Backlog Task &amp; ID</t>
   </si>
@@ -227,10 +227,10 @@
     <t>User Story #</t>
   </si>
   <si>
-    <t xml:space="preserve">Return list from database in order of </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return list from database based on </t>
+    <t xml:space="preserve">Return list from database </t>
+  </si>
+  <si>
+    <t>Return results from database, nearest to location</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,12 +275,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,7 +330,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,7 +647,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +1028,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C22" t="s">
@@ -1100,7 +1093,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C26" t="s">

</xml_diff>